<commit_message>
Updates for video links, incorporated
</commit_message>
<xml_diff>
--- a/Video_Consistency.xlsx
+++ b/Video_Consistency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiki/Documents/Personal/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F696E427-F6D0-2C4D-9513-7BEC37F99EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC26A9A-8E7C-1F4C-833B-A84FE5730676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2460" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{372ECBC3-F3BA-9D4F-BAFB-5E677E6AD54B}"/>
+    <workbookView xWindow="-2460" yWindow="-21140" windowWidth="38400" windowHeight="19720" activeTab="1" xr2:uid="{372ECBC3-F3BA-9D4F-BAFB-5E677E6AD54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="978">
   <si>
     <t>Disk</t>
   </si>
@@ -2970,6 +2970,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Spelling is correct. Uploaded On Server</t>
   </si>
 </sst>
 </file>
@@ -3415,8 +3418,8 @@
   <dimension ref="A1:E294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A269" sqref="A269"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -5934,12 +5937,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4395DED-9881-3540-8E28-77BAE65B573D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U295"/>
+  <dimension ref="A1:V295"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A163"/>
+      <selection pane="bottomLeft" activeCell="V49" sqref="V49:V163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5963,7 +5966,8 @@
     <col min="18" max="18" width="54.5" customWidth="1"/>
     <col min="19" max="19" width="45.5" customWidth="1"/>
     <col min="20" max="20" width="23.6640625" customWidth="1"/>
-    <col min="21" max="21" width="110" customWidth="1"/>
+    <col min="21" max="21" width="53.6640625" customWidth="1"/>
+    <col min="22" max="22" width="106.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
@@ -8689,7 +8693,7 @@
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Bhago Re Jag Se Ab Bhago.mp4' where Shabd1_ID = 801</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>811</v>
       </c>
@@ -8739,8 +8743,15 @@
         <f>IF(COUNTIF(R2:R295, C49), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U49" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="V49" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U49,".mp4' where Shabd1_ID = ",A49)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Satguru Pyare Ne Sunaee Jugat Nirali Ho.mp4' where Shabd1_ID = 811</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>816</v>
       </c>
@@ -8787,8 +8798,9 @@
         <f>IF(COUNTIF(R2:R295, C50), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V50" s="9"/>
+    </row>
+    <row r="51" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>842</v>
       </c>
@@ -8842,12 +8854,8 @@
         <f>IF(COUNTIF(R2:R295, C51), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U51" t="str">
-        <f t="shared" ref="U51:U52" si="11">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S51,"' where Shabd1_ID = ",A51)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Bin Satguru Didar Tadap Rahi Man Mein.mp4' where Shabd1_ID = 842</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>848</v>
       </c>
@@ -8898,12 +8906,8 @@
         <f>IF(COUNTIF(R2:R295, C52), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U52" t="str">
-        <f t="shared" si="11"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Binti Gave Das Anokha.mp4' where Shabd1_ID = 848</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:22" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>854</v>
       </c>
@@ -8950,8 +8954,9 @@
         <f>IF(COUNTIF(R2:R295, C53), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V53" s="9"/>
+    </row>
+    <row r="54" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>863</v>
       </c>
@@ -8998,19 +9003,18 @@
         <v>53</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" ref="S54:S55" si="12">_xlfn.CONCAT("Video/Poetry/",R54,".mp4")</f>
+        <f t="shared" ref="S54:S55" si="11">_xlfn.CONCAT("Video/Poetry/",R54,".mp4")</f>
         <v>Video/Poetry/Binti Karoon Pukar Pukari.mp4</v>
       </c>
       <c r="T54" t="str">
         <f>IF(COUNTIF(R2:R295, C54), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U54" t="str">
-        <f t="shared" ref="U54:U55" si="13">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S54,"' where Shabd1_ID = ",A54)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Binti Karoon Pukar Pukari.mp4' where Shabd1_ID = 863</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U54" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>887</v>
       </c>
@@ -9057,19 +9061,18 @@
         <v>54</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Video/Poetry/Bol Ri Radha Pyari Bansi.mp4</v>
       </c>
       <c r="T55" t="str">
         <f>IF(COUNTIF(R2:R295, C55), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U55" t="str">
-        <f t="shared" si="13"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Bol Ri Radha Pyari Bansi.mp4' where Shabd1_ID = 887</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>889</v>
       </c>
@@ -9116,8 +9119,9 @@
         <f>IF(COUNTIF(R2:R295, C56), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V56" s="9"/>
+    </row>
+    <row r="57" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>912</v>
       </c>
@@ -9164,19 +9168,15 @@
         <v>56</v>
       </c>
       <c r="S57" t="str">
-        <f t="shared" ref="S57:S65" si="14">_xlfn.CONCAT("Video/Poetry/",R57,".mp4")</f>
+        <f t="shared" ref="S57:S65" si="12">_xlfn.CONCAT("Video/Poetry/",R57,".mp4")</f>
         <v>Video/Poetry/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp4</v>
       </c>
       <c r="T57" t="str">
         <f>IF(COUNTIF(R2:R295, C57), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U57" t="str">
-        <f t="shared" ref="U57:U65" si="15">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S57,"' where Shabd1_ID = ",A57)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp4' where Shabd1_ID = 912</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>918</v>
       </c>
@@ -9223,19 +9223,15 @@
         <v>57</v>
       </c>
       <c r="S58" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Chalo Ri Sakhi Mil Aarat Gaven.mp4</v>
       </c>
       <c r="T58" t="str">
         <f>IF(COUNTIF(R2:R295, C58), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U58" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Chalo Ri Sakhi Mil Aarat Gaven.mp4' where Shabd1_ID = 918</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>931</v>
       </c>
@@ -9282,19 +9278,18 @@
         <v>58</v>
       </c>
       <c r="S59" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Charan Guru Badhat Hiye Anurag.mp4</v>
       </c>
       <c r="T59" t="str">
         <f>IF(COUNTIF(R2:R295, C59), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U59" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Charan Guru Badhat Hiye Anurag.mp4' where Shabd1_ID = 931</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U59" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>935</v>
       </c>
@@ -9341,19 +9336,15 @@
         <v>59</v>
       </c>
       <c r="S60" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Charan Guru Hirdey Dhar Rahi.mp4</v>
       </c>
       <c r="T60" t="str">
         <f>IF(COUNTIF(R2:R295, C60), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U60" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Charan Guru Hirdey Dhar Rahi.mp4' where Shabd1_ID = 935</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>938</v>
       </c>
@@ -9400,19 +9391,18 @@
         <v>60</v>
       </c>
       <c r="S61" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Charan Ur Dharo Radha Pyari.mp4</v>
       </c>
       <c r="T61" t="str">
         <f>IF(COUNTIF(R2:R295, C61), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U61" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Charan Ur Dharo Radha Pyari.mp4' where Shabd1_ID = 938</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>939</v>
       </c>
@@ -9459,19 +9449,18 @@
         <v>61</v>
       </c>
       <c r="S62" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Chauka Bartan Kiya Achambhi.mp4</v>
       </c>
       <c r="T62" t="str">
         <f>IF(COUNTIF(R2:R295, C62), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U62" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Chauka Bartan Kiya Achambhi.mp4' where Shabd1_ID = 939</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>940</v>
       </c>
@@ -9518,19 +9507,18 @@
         <v>62</v>
       </c>
       <c r="S63" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Chet Chalo Yeh Sab Janjal.mp4</v>
       </c>
       <c r="T63" t="str">
         <f>IF(COUNTIF(R2:R295, C63), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U63" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Chet Chalo Yeh Sab Janjal.mp4' where Shabd1_ID = 940</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>944</v>
       </c>
@@ -9577,19 +9565,18 @@
         <v>63</v>
       </c>
       <c r="S64" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Cheto Mere Pyare Tere Bhale Ki Kahoon.mp4</v>
       </c>
       <c r="T64" t="str">
         <f>IF(COUNTIF(R2:R295, C64), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U64" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Cheto Mere Pyare Tere Bhale Ki Kahoon.mp4' where Shabd1_ID = 944</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U64" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>945</v>
       </c>
@@ -9636,19 +9623,18 @@
         <v>64</v>
       </c>
       <c r="S65" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>Video/Poetry/Cheto Re Ghar Ghat Samharo.mp4</v>
       </c>
       <c r="T65" t="str">
         <f>IF(COUNTIF(R2:R295, C65), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U65" t="str">
-        <f t="shared" si="15"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Cheto Re Ghar Ghat Samharo.mp4' where Shabd1_ID = 945</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U65" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>946</v>
       </c>
@@ -9698,8 +9684,15 @@
         <f>IF(COUNTIF(R2:R295, C66), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U66" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="V66" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U66,".mp4' where Shabd1_ID = ",A66)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Phaagun Ki Ritu Aaee Sakhi Aaj Guru Sang Phaag Racho.mp4' where Shabd1_ID = 946</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>954</v>
       </c>
@@ -9753,12 +9746,11 @@
         <f>IF(COUNTIF(R2:R295, C67), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U67" t="str">
-        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = '",S67,"' where Shabd1_ID = ",A67)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Chunar Meri Maili Bhayee.mp4' where Shabd1_ID = 954</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U67" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>976</v>
       </c>
@@ -9808,8 +9800,15 @@
         <f>IF(COUNTIF(R2:R295, C68), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U68" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="V68" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U68,".mp4' where Shabd1_ID = ",A68)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Phaagun Ki Ritu Aaee Sakhi Mil Satguru Khelo Holi.mp4' where Shabd1_ID = 976</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>977</v>
       </c>
@@ -9856,19 +9855,18 @@
         <v>68</v>
       </c>
       <c r="S69" t="str">
-        <f t="shared" ref="S69:S70" si="16">_xlfn.CONCAT("Video/Poetry/",R69,".mp4")</f>
+        <f t="shared" ref="S69:S70" si="13">_xlfn.CONCAT("Video/Poetry/",R69,".mp4")</f>
         <v>Video/Poetry/Darash De Aaj Bandhao Dheer.mp4</v>
       </c>
       <c r="T69" t="str">
         <f>IF(COUNTIF(R2:R295, C69), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U69" t="str">
-        <f t="shared" ref="U69:U70" si="17">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S69,"' where Shabd1_ID = ",A69)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Darash De Aaj Bandhao Dheer.mp4' where Shabd1_ID = 977</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U69" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>978</v>
       </c>
@@ -9915,7 +9913,7 @@
         <v>69</v>
       </c>
       <c r="S70" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>Video/Poetry/Darash Guru Tadap Raha Man Mor.mp4</v>
       </c>
       <c r="T70" t="str">
@@ -9923,11 +9921,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U70" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="U69:U70" si="14">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S70,"' where Shabd1_ID = ",A70)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Darash Guru Tadap Raha Man Mor.mp4' where Shabd1_ID = 978</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>979</v>
       </c>
@@ -9977,8 +9975,15 @@
         <f>IF(COUNTIF(R2:R295, C71), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U71" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="V71" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U71,".mp4' where Shabd1_ID = ",A71)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Nirkho Nirkho Sakhi Ritu Aaee Basant.mp4' where Shabd1_ID = 979</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>985</v>
       </c>
@@ -10037,7 +10042,7 @@
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dard Dukhi Jiyara Nit Tarse.mp4' where Shabd1_ID = 985</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>998</v>
       </c>
@@ -10084,8 +10089,15 @@
         <f>IF(COUNTIF(R2:R295, C73), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U73" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="V73" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U73,".mp4' where Shabd1_ID = ",A73)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Sindh Se Aaee Soorat Nar.mp4' where Shabd1_ID = 998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1001</v>
       </c>
@@ -10132,7 +10144,7 @@
         <v>73</v>
       </c>
       <c r="S74" t="str">
-        <f t="shared" ref="S74:S101" si="18">_xlfn.CONCAT("Video/Poetry/",R74,".mp4")</f>
+        <f t="shared" ref="S74:S101" si="15">_xlfn.CONCAT("Video/Poetry/",R74,".mp4")</f>
         <v>Video/Poetry/Darshan Ki Pyas Ghaneri.mp4</v>
       </c>
       <c r="T74" t="str">
@@ -10140,11 +10152,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U74" t="str">
-        <f t="shared" ref="U74:U101" si="19">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S74,"' where Shabd1_ID = ",A74)</f>
+        <f t="shared" ref="U74:U101" si="16">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S74,"' where Shabd1_ID = ",A74)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Darshan Ki Pyas Ghaneri.mp4' where Shabd1_ID = 1001</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1003</v>
       </c>
@@ -10194,7 +10206,7 @@
         <v>74</v>
       </c>
       <c r="S75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Daya Guru Kya Karoon Varnan.mp4</v>
       </c>
       <c r="T75" t="str">
@@ -10202,11 +10214,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Daya Guru Kya Karoon Varnan.mp4' where Shabd1_ID = 1003</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1014</v>
       </c>
@@ -10256,7 +10268,7 @@
         <v>75</v>
       </c>
       <c r="S76" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dekhan Chali Basant Agam Ghar.mp4</v>
       </c>
       <c r="T76" t="str">
@@ -10264,11 +10276,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U76" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dekhan Chali Basant Agam Ghar.mp4' where Shabd1_ID = 1014</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1018</v>
       </c>
@@ -10315,7 +10327,7 @@
         <v>76</v>
       </c>
       <c r="S77" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dekho Dekho Sakhi Ab Chal Basant.mp4</v>
       </c>
       <c r="T77" t="str">
@@ -10323,11 +10335,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U77" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dekho Dekho Sakhi Ab Chal Basant.mp4' where Shabd1_ID = 1018</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1019</v>
       </c>
@@ -10374,7 +10386,7 @@
         <v>77</v>
       </c>
       <c r="S78" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dekho Sab Jag Jat Baha.mp4</v>
       </c>
       <c r="T78" t="str">
@@ -10382,11 +10394,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U78" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dekho Sab Jag Jat Baha.mp4' where Shabd1_ID = 1019</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1020</v>
       </c>
@@ -10433,7 +10445,7 @@
         <v>78</v>
       </c>
       <c r="S79" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dev Ri Sakhi Mohin Umang Badhaee.mp4</v>
       </c>
       <c r="T79" t="str">
@@ -10441,11 +10453,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U79" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dev Ri Sakhi Mohin Umang Badhaee.mp4' where Shabd1_ID = 1020</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1032</v>
       </c>
@@ -10492,7 +10504,7 @@
         <v>79</v>
       </c>
       <c r="S80" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dham Apne Chalo Bhai.mp4</v>
       </c>
       <c r="T80" t="str">
@@ -10500,7 +10512,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U80" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dham Apne Chalo Bhai.mp4' where Shabd1_ID = 1032</v>
       </c>
     </row>
@@ -10548,7 +10560,7 @@
         <v>80</v>
       </c>
       <c r="S81" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dhiraj Dharana Mat Ghabrana.mp4</v>
       </c>
       <c r="T81" t="str">
@@ -10556,7 +10568,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U81" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dhiraj Dharana Mat Ghabrana.mp4' where Shabd1_ID = 1034</v>
       </c>
     </row>
@@ -10607,7 +10619,7 @@
         <v>81</v>
       </c>
       <c r="S82" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dhiraj Dharo Bachan Guru Gaho.mp4</v>
       </c>
       <c r="T82" t="str">
@@ -10615,7 +10627,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U82" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dhiraj Dharo Bachan Guru Gaho.mp4' where Shabd1_ID = 1119</v>
       </c>
     </row>
@@ -10666,7 +10678,7 @@
         <v>82</v>
       </c>
       <c r="S83" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dhokha Mat Khana Jag Aay Piyare.mp4</v>
       </c>
       <c r="T83" t="str">
@@ -10674,7 +10686,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U83" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dhokha Mat Khana Jag Aay Piyare.mp4' where Shabd1_ID = 1129</v>
       </c>
     </row>
@@ -10725,7 +10737,7 @@
         <v>83</v>
       </c>
       <c r="S84" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dhun Mein Ab Surat Lagao.mp4</v>
       </c>
       <c r="T84" t="str">
@@ -10733,7 +10745,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U84" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dhun Mein Ab Surat Lagao.mp4' where Shabd1_ID = 1250</v>
       </c>
     </row>
@@ -10784,7 +10796,7 @@
         <v>84</v>
       </c>
       <c r="S85" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Dhun Sun Kar Man Samajhaee.mp4</v>
       </c>
       <c r="T85" t="str">
@@ -10792,7 +10804,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U85" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Dhun Sun Kar Man Samajhaee.mp4' where Shabd1_ID = 1251</v>
       </c>
     </row>
@@ -10843,7 +10855,7 @@
         <v>85</v>
       </c>
       <c r="S86" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Diwala Poojen Jeev Ajan.mp4</v>
       </c>
       <c r="T86" t="str">
@@ -10851,7 +10863,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U86" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Diwala Poojen Jeev Ajan.mp4' where Shabd1_ID = 1252</v>
       </c>
     </row>
@@ -10902,7 +10914,7 @@
         <v>86</v>
       </c>
       <c r="S87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Gagan Mein Bajat Aaj Badhaee.mp4</v>
       </c>
       <c r="T87" t="str">
@@ -10910,7 +10922,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Gagan Mein Bajat Aaj Badhaee.mp4' where Shabd1_ID = 1254</v>
       </c>
     </row>
@@ -10958,7 +10970,7 @@
         <v>87</v>
       </c>
       <c r="S88" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Gaoon Arti Lekar Thali.mp4</v>
       </c>
       <c r="T88" t="str">
@@ -10966,7 +10978,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U88" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Gaoon Arti Lekar Thali.mp4' where Shabd1_ID = 1260</v>
       </c>
     </row>
@@ -11017,7 +11029,7 @@
         <v>88</v>
       </c>
       <c r="S89" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Gave Arti Sevak Poora.mp4</v>
       </c>
       <c r="T89" t="str">
@@ -11025,7 +11037,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U89" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Gave Arti Sevak Poora.mp4' where Shabd1_ID = 1270</v>
       </c>
     </row>
@@ -11076,7 +11088,7 @@
         <v>89</v>
       </c>
       <c r="S90" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Ghat Mein Kheloon Ab Basant.mp4</v>
       </c>
       <c r="T90" t="str">
@@ -11084,7 +11096,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U90" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Ghat Mein Kheloon Ab Basant.mp4' where Shabd1_ID = 1278</v>
       </c>
     </row>
@@ -11135,7 +11147,7 @@
         <v>90</v>
       </c>
       <c r="S91" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Aarat Main Karne Aaee.mp4</v>
       </c>
       <c r="T91" t="str">
@@ -11143,7 +11155,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U91" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Aarat Main Karne Aaee.mp4' where Shabd1_ID = 1279</v>
       </c>
     </row>
@@ -11194,7 +11206,7 @@
         <v>91</v>
       </c>
       <c r="S92" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Aarat Tu Kar Le Sajni.mp4</v>
       </c>
       <c r="T92" t="str">
@@ -11202,7 +11214,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U92" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Aarat Tu Kar Le Sajni.mp4' where Shabd1_ID = 1281</v>
       </c>
     </row>
@@ -11253,7 +11265,7 @@
         <v>92</v>
       </c>
       <c r="S93" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Bin Kabhi Na Utre Par.mp4</v>
       </c>
       <c r="T93" t="str">
@@ -11261,7 +11273,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U93" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Bin Kabhi Na Utre Par.mp4' where Shabd1_ID = 1287</v>
       </c>
     </row>
@@ -11312,7 +11324,7 @@
         <v>93</v>
       </c>
       <c r="S94" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Charan Girah Mere Aaye.mp4</v>
       </c>
       <c r="T94" t="str">
@@ -11320,7 +11332,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U94" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Charan Girah Mere Aaye.mp4' where Shabd1_ID = 1288</v>
       </c>
     </row>
@@ -11371,7 +11383,7 @@
         <v>94</v>
       </c>
       <c r="S95" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Charan Pakad Dradh Bhai.mp4</v>
       </c>
       <c r="T95" t="str">
@@ -11379,7 +11391,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U95" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Charan Pakad Dradh Bhai.mp4' where Shabd1_ID = 1292</v>
       </c>
     </row>
@@ -11430,7 +11442,7 @@
         <v>95</v>
       </c>
       <c r="S96" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Dhara Sis Par Hath Man Kyon Soch Kare.mp4</v>
       </c>
       <c r="T96" t="str">
@@ -11438,11 +11450,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U96" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Dhara Sis Par Hath Man Kyon Soch Kare.mp4' where Shabd1_ID = 1293</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1294</v>
       </c>
@@ -11489,7 +11501,7 @@
         <v>96</v>
       </c>
       <c r="S97" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Dhyan Dharo Tum Man Mein.mp4</v>
       </c>
       <c r="T97" t="str">
@@ -11497,11 +11509,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U97" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Dhyan Dharo Tum Man Mein.mp4' where Shabd1_ID = 1294</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1298</v>
       </c>
@@ -11548,7 +11560,7 @@
         <v>97</v>
       </c>
       <c r="S98" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Ka Agam Roop Main Dekha.mp4</v>
       </c>
       <c r="T98" t="str">
@@ -11556,11 +11568,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U98" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Ka Agam Roop Main Dekha.mp4' where Shabd1_ID = 1298</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1300</v>
       </c>
@@ -11607,7 +11619,7 @@
         <v>98</v>
       </c>
       <c r="S99" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Ka Dhyan Kar Pyare.mp4</v>
       </c>
       <c r="T99" t="str">
@@ -11615,11 +11627,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U99" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Ka Dhyan Kar Pyare.mp4' where Shabd1_ID = 1300</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1303</v>
       </c>
@@ -11666,7 +11678,7 @@
         <v>99</v>
       </c>
       <c r="S100" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Karo Khoj Kar Bhai.mp4</v>
       </c>
       <c r="T100" t="str">
@@ -11674,11 +11686,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U100" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Karo Khoj Kar Bhai.mp4' where Shabd1_ID = 1303</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1304</v>
       </c>
@@ -11725,7 +11737,7 @@
         <v>100</v>
       </c>
       <c r="S101" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>Video/Poetry/Guru Ke Daras Par Main Balihari.mp4</v>
       </c>
       <c r="T101" t="str">
@@ -11733,11 +11745,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U101" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Ke Daras Par Main Balihari.mp4' where Shabd1_ID = 1304</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>1316</v>
       </c>
@@ -11787,8 +11799,9 @@
         <f>IF(COUNTIF(R2:R295, C102), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="103" spans="1:21" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="V102" s="9"/>
+    </row>
+    <row r="103" spans="1:22" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A103" s="12">
         <v>1318</v>
       </c>
@@ -11838,8 +11851,9 @@
         <f>IF(COUNTIF(R2:R295, C103), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="104" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V103" s="9"/>
+    </row>
+    <row r="104" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1321</v>
       </c>
@@ -11886,7 +11900,7 @@
         <v>103</v>
       </c>
       <c r="S104" t="str">
-        <f t="shared" ref="S104:S111" si="20">_xlfn.CONCAT("Video/Poetry/",R104,".mp4")</f>
+        <f t="shared" ref="S104:S111" si="17">_xlfn.CONCAT("Video/Poetry/",R104,".mp4")</f>
         <v>Video/Poetry/Guru Ki Kar Har Dam Pooja.mp4</v>
       </c>
       <c r="T104" t="str">
@@ -11894,11 +11908,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U104" t="str">
-        <f t="shared" ref="U104:U111" si="21">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S104,"' where Shabd1_ID = ",A104)</f>
+        <f t="shared" ref="U104:U111" si="18">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S104,"' where Shabd1_ID = ",A104)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Ki Kar Har Dam Pooja.mp4' where Shabd1_ID = 1321</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1355</v>
       </c>
@@ -11945,7 +11959,7 @@
         <v>104</v>
       </c>
       <c r="S105" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Ki Mauj Raho Tum Dhar.mp4</v>
       </c>
       <c r="T105" t="str">
@@ -11953,11 +11967,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U105" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Ki Mauj Raho Tum Dhar.mp4' where Shabd1_ID = 1355</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1357</v>
       </c>
@@ -12004,7 +12018,7 @@
         <v>105</v>
       </c>
       <c r="S106" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Main Gunahagar Ati Bhari.mp4</v>
       </c>
       <c r="T106" t="str">
@@ -12012,11 +12026,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U106" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Main Gunahagar Ati Bhari.mp4' where Shabd1_ID = 1357</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1358</v>
       </c>
@@ -12063,7 +12077,7 @@
         <v>106</v>
       </c>
       <c r="S107" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Mere Data Main Bhai Dasi.mp4</v>
       </c>
       <c r="T107" t="str">
@@ -12071,11 +12085,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U107" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Mere Data Main Bhai Dasi.mp4' where Shabd1_ID = 1358</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1359</v>
       </c>
@@ -12122,7 +12136,7 @@
         <v>107</v>
       </c>
       <c r="S108" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Mere Pragate Jag Mein Aay.mp4</v>
       </c>
       <c r="T108" t="str">
@@ -12130,11 +12144,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U108" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Mere Pragate Jag Mein Aay.mp4' where Shabd1_ID = 1359</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1360</v>
       </c>
@@ -12181,7 +12195,7 @@
         <v>108</v>
       </c>
       <c r="S109" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Mile Ami Ras Data.mp4</v>
       </c>
       <c r="T109" t="str">
@@ -12189,11 +12203,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U109" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Mile Ami Ras Data.mp4' where Shabd1_ID = 1360</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1363</v>
       </c>
@@ -12240,7 +12254,7 @@
         <v>109</v>
       </c>
       <c r="S110" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Mohin Apna Roop Dikhao.mp4</v>
       </c>
       <c r="T110" t="str">
@@ -12248,11 +12262,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U110" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Mohin Apna Roop Dikhao.mp4' where Shabd1_ID = 1363</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1366</v>
       </c>
@@ -12299,7 +12313,7 @@
         <v>110</v>
       </c>
       <c r="S111" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>Video/Poetry/Guru Moorat Mere Man Bas Gaiyan.mp4</v>
       </c>
       <c r="T111" t="str">
@@ -12307,11 +12321,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U111" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Moorat Mere Man Bas Gaiyan.mp4' where Shabd1_ID = 1366</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <v>1367</v>
       </c>
@@ -12361,8 +12375,15 @@
         <f>IF(COUNTIF(R2:R295, C112), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="113" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U112" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="V112" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U112,".mp4' where Shabd1_ID = ",A112)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Mili Nar Deh Yeh Tum Ko.mp4' where Shabd1_ID = 1367</v>
+      </c>
+    </row>
+    <row r="113" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1368</v>
       </c>
@@ -12409,7 +12430,7 @@
         <v>112</v>
       </c>
       <c r="S113" t="str">
-        <f t="shared" ref="S113:S120" si="22">_xlfn.CONCAT("Video/Poetry/",R113,".mp4")</f>
+        <f t="shared" ref="S113:S120" si="19">_xlfn.CONCAT("Video/Poetry/",R113,".mp4")</f>
         <v>Video/Poetry/Guru Pyare Ka Rang Ati Nirmal.mp4</v>
       </c>
       <c r="T113" t="str">
@@ -12417,11 +12438,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U113" t="str">
-        <f t="shared" ref="U113:U120" si="23">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S113,"' where Shabd1_ID = ",A113)</f>
+        <f t="shared" ref="U113:U120" si="20">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S113,"' where Shabd1_ID = ",A113)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Ka Rang Ati Nirmal.mp4' where Shabd1_ID = 1368</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1369</v>
       </c>
@@ -12468,7 +12489,7 @@
         <v>113</v>
       </c>
       <c r="S114" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp4</v>
       </c>
       <c r="T114" t="str">
@@ -12476,11 +12497,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U114" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp4' where Shabd1_ID = 1369</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1381</v>
       </c>
@@ -12527,7 +12548,7 @@
         <v>114</v>
       </c>
       <c r="S115" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Pyare Karen Aaj Jagat Uddhar.mp4</v>
       </c>
       <c r="T115" t="str">
@@ -12535,11 +12556,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U115" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Karen Aaj Jagat Uddhar.mp4' where Shabd1_ID = 1381</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1384</v>
       </c>
@@ -12586,7 +12607,7 @@
         <v>115</v>
       </c>
       <c r="S116" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Pyare Ke Darshan Karat Rahoon.mp4</v>
       </c>
       <c r="T116" t="str">
@@ -12594,11 +12615,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U116" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Ke Darshan Karat Rahoon.mp4' where Shabd1_ID = 1384</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1385</v>
       </c>
@@ -12645,7 +12666,7 @@
         <v>116</v>
       </c>
       <c r="S117" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Pyare Ke Sang Pyari Khelo Phaag.mp4</v>
       </c>
       <c r="T117" t="str">
@@ -12653,11 +12674,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U117" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Ke Sang Pyari Khelo Phaag.mp4' where Shabd1_ID = 1385</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1388</v>
       </c>
@@ -12704,7 +12725,7 @@
         <v>117</v>
       </c>
       <c r="S118" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Pyare Ki Chhavi Man Mohan.mp4</v>
       </c>
       <c r="T118" t="str">
@@ -12712,11 +12733,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U118" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Ki Chhavi Man Mohan.mp4' where Shabd1_ID = 1388</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1393</v>
       </c>
@@ -12763,7 +12784,7 @@
         <v>118</v>
       </c>
       <c r="S119" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Pyare Ki Mauj Raho Tum Dhar.mp4</v>
       </c>
       <c r="T119" t="str">
@@ -12771,11 +12792,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U119" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Pyare Ki Mauj Raho Tum Dhar.mp4' where Shabd1_ID = 1393</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1394</v>
       </c>
@@ -12822,7 +12843,7 @@
         <v>119</v>
       </c>
       <c r="S120" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>Video/Poetry/Guru Sang Kheloon Nis Din Pas.mp4</v>
       </c>
       <c r="T120" t="str">
@@ -12830,11 +12851,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U120" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Sang Kheloon Nis Din Pas.mp4' where Shabd1_ID = 1394</v>
       </c>
     </row>
-    <row r="121" spans="1:21" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A121" s="12">
         <v>1395</v>
       </c>
@@ -12881,8 +12902,9 @@
         <f>IF(COUNTIF(R2:R295, C121), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="122" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V121" s="9"/>
+    </row>
+    <row r="122" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1396</v>
       </c>
@@ -12929,7 +12951,7 @@
         <v>121</v>
       </c>
       <c r="S122" t="str">
-        <f t="shared" ref="S122:S124" si="24">_xlfn.CONCAT("Video/Poetry/",R122,".mp4")</f>
+        <f t="shared" ref="S122:S124" si="21">_xlfn.CONCAT("Video/Poetry/",R122,".mp4")</f>
         <v>Video/Poetry/Guru Tarenge Ham Jani.mp4</v>
       </c>
       <c r="T122" t="str">
@@ -12937,11 +12959,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U122" t="str">
-        <f t="shared" ref="U122:U124" si="25">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S122,"' where Shabd1_ID = ",A122)</f>
+        <f t="shared" ref="U122:U124" si="22">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S122,"' where Shabd1_ID = ",A122)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Guru Tarenge Ham Jani.mp4' where Shabd1_ID = 1396</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1407</v>
       </c>
@@ -12988,7 +13010,7 @@
         <v>122</v>
       </c>
       <c r="S123" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>Video/Poetry/He Guru Main Tere Didar Ka Aashik Jo Hua.mp4</v>
       </c>
       <c r="T123" t="str">
@@ -12996,11 +13018,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U123" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/He Guru Main Tere Didar Ka Aashik Jo Hua.mp4' where Shabd1_ID = 1407</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1410</v>
       </c>
@@ -13047,7 +13069,7 @@
         <v>123</v>
       </c>
       <c r="S124" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>Video/Poetry/He Mere Pyare Satguru Mohin Darshan Dije.mp4</v>
       </c>
       <c r="T124" t="str">
@@ -13055,11 +13077,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U124" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/He Mere Pyare Satguru Mohin Darshan Dije.mp4' where Shabd1_ID = 1410</v>
       </c>
     </row>
-    <row r="125" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>1445</v>
       </c>
@@ -13109,8 +13131,15 @@
         <f>IF(COUNTIF(R2:R295, C125), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="126" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U125" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="V125" s="9" t="str">
+        <f t="shared" ref="V125:V128" si="23">_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U125,".mp4' where Shabd1_ID = ",A125)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/He Guru Main Tere Didar Ka Aashik Jo Hua.mp4' where Shabd1_ID = 1445</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>1446</v>
       </c>
@@ -13157,8 +13186,15 @@
         <f>IF(COUNTIF(R2:R295, C126), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="127" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U126" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="V126" s="9" t="str">
+        <f t="shared" si="23"/>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Arsh Par Pahunch Kar Main Dekha Noor.mp4' where Shabd1_ID = 1446</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>1447</v>
       </c>
@@ -13208,8 +13244,15 @@
         <f>IF(COUNTIF(R2:R295, C127), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="128" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="U127" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="V127" s="9" t="str">
+        <f t="shared" si="23"/>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Nij Roop Poore Satguru Ka.mp4' where Shabd1_ID = 1447</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>1448</v>
       </c>
@@ -13259,6 +13302,13 @@
         <f>IF(COUNTIF(R2:R295, C128), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
+      <c r="U128" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="V128" s="9" t="str">
+        <f t="shared" si="23"/>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Surt Aawaz Ko Pakad Ke.mp4' where Shabd1_ID = 1448</v>
+      </c>
     </row>
     <row r="129" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
@@ -13307,16 +13357,15 @@
         <v>128</v>
       </c>
       <c r="S129" t="str">
-        <f t="shared" ref="S129:S146" si="26">_xlfn.CONCAT("Video/Poetry/",R129,".mp4")</f>
+        <f t="shared" ref="S129:S146" si="24">_xlfn.CONCAT("Video/Poetry/",R129,".mp4")</f>
         <v>Video/Poetry/Holi Khel Na Jane Bawariya.mp4</v>
       </c>
       <c r="T129" t="str">
         <f>IF(COUNTIF(R2:R295, C129), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U129" t="str">
-        <f t="shared" ref="U129:U146" si="27">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S129,"' where Shabd1_ID = ",A129)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Holi Khel Na Jane Bawariya.mp4' where Shabd1_ID = 1468</v>
+      <c r="U129" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="130" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
@@ -13366,16 +13415,15 @@
         <v>129</v>
       </c>
       <c r="S130" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp4</v>
       </c>
       <c r="T130" t="str">
         <f>IF(COUNTIF(R2:R295, C130), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U130" t="str">
-        <f t="shared" si="27"/>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp4' where Shabd1_ID = 1474</v>
+      <c r="U130" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="131" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
@@ -13425,7 +13473,7 @@
         <v>130</v>
       </c>
       <c r="S131" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jab Se Main Dekha Radhasoami Ka Mukhada.mp4</v>
       </c>
       <c r="T131" t="str">
@@ -13433,7 +13481,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U131" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="U129:U146" si="25">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S131,"' where Shabd1_ID = ",A131)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jab Se Main Dekha Radhasoami Ka Mukhada.mp4' where Shabd1_ID = 1476</v>
       </c>
     </row>
@@ -13484,7 +13532,7 @@
         <v>131</v>
       </c>
       <c r="S132" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jagat Jeev Sab Holi Poojen.mp4</v>
       </c>
       <c r="T132" t="str">
@@ -13492,7 +13540,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U132" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jagat Jeev Sab Holi Poojen.mp4' where Shabd1_ID = 1478</v>
       </c>
     </row>
@@ -13543,7 +13591,7 @@
         <v>132</v>
       </c>
       <c r="S133" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jagi Hai Umang Mere Hiye Mein.mp4</v>
       </c>
       <c r="T133" t="str">
@@ -13551,7 +13599,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U133" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jagi Hai Umang Mere Hiye Mein.mp4' where Shabd1_ID = 1480</v>
       </c>
     </row>
@@ -13602,7 +13650,7 @@
         <v>133</v>
       </c>
       <c r="S134" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jago Re Yehan Kab Lag Sona.mp4</v>
       </c>
       <c r="T134" t="str">
@@ -13610,7 +13658,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U134" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jago Re Yehan Kab Lag Sona.mp4' where Shabd1_ID = 1483</v>
       </c>
     </row>
@@ -13661,7 +13709,7 @@
         <v>134</v>
       </c>
       <c r="S135" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jeev Chitawan Aaye Radhasoami.mp4</v>
       </c>
       <c r="T135" t="str">
@@ -13669,7 +13717,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U135" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jeev Chitawan Aaye Radhasoami.mp4' where Shabd1_ID = 1488</v>
       </c>
     </row>
@@ -13720,7 +13768,7 @@
         <v>135</v>
       </c>
       <c r="S136" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jeev Chitaya Rahe Radhasoami.mp4</v>
       </c>
       <c r="T136" t="str">
@@ -13728,7 +13776,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U136" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jeev Chitaya Rahe Radhasoami.mp4' where Shabd1_ID = 1504</v>
       </c>
     </row>
@@ -13779,7 +13827,7 @@
         <v>136</v>
       </c>
       <c r="S137" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jeev Ubaran Jag Mein Aaye.mp4</v>
       </c>
       <c r="T137" t="str">
@@ -13787,7 +13835,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U137" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jeev Ubaran Jag Mein Aaye.mp4' where Shabd1_ID = 1506</v>
       </c>
     </row>
@@ -13838,7 +13886,7 @@
         <v>137</v>
       </c>
       <c r="S138" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jo Mere Preetam Se Preet Kare.mp4</v>
       </c>
       <c r="T138" t="str">
@@ -13846,7 +13894,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U138" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jo Mere Preetam Se Preet Kare.mp4' where Shabd1_ID = 1534</v>
       </c>
     </row>
@@ -13897,7 +13945,7 @@
         <v>138</v>
       </c>
       <c r="S139" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp4</v>
       </c>
       <c r="T139" t="str">
@@ -13905,7 +13953,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U139" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp4' where Shabd1_ID = 1537</v>
       </c>
     </row>
@@ -13956,7 +14004,7 @@
         <v>139</v>
       </c>
       <c r="S140" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Kaise Karoon Charan Mein Binti.mp4</v>
       </c>
       <c r="T140" t="str">
@@ -13964,7 +14012,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U140" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kaise Karoon Charan Mein Binti.mp4' where Shabd1_ID = 1538</v>
       </c>
     </row>
@@ -14015,7 +14063,7 @@
         <v>140</v>
       </c>
       <c r="S141" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Kaisi Karoon Kasak Uthi Bhari.mp4</v>
       </c>
       <c r="T141" t="str">
@@ -14023,7 +14071,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U141" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kaisi Karoon Kasak Uthi Bhari.mp4' where Shabd1_ID = 1543</v>
       </c>
     </row>
@@ -14074,7 +14122,7 @@
         <v>141</v>
       </c>
       <c r="S142" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Kal Ne Jagat Ajab Bharmaya.mp4</v>
       </c>
       <c r="T142" t="str">
@@ -14082,7 +14130,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U142" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kal Ne Jagat Ajab Bharmaya.mp4' where Shabd1_ID = 1547</v>
       </c>
     </row>
@@ -14133,7 +14181,7 @@
         <v>142</v>
       </c>
       <c r="S143" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Karat Hoon Pukar Aaj Suniye Guhar.mp4</v>
       </c>
       <c r="T143" t="str">
@@ -14141,7 +14189,7 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U143" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Karat Hoon Pukar Aaj Suniye Guhar.mp4' where Shabd1_ID = 1549</v>
       </c>
     </row>
@@ -14192,7 +14240,7 @@
         <v>143</v>
       </c>
       <c r="S144" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Kare Aarata Sevak Bhola.mp4</v>
       </c>
       <c r="T144" t="str">
@@ -14200,11 +14248,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U144" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kare Aarata Sevak Bhola.mp4' where Shabd1_ID = 1551</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1557</v>
       </c>
@@ -14251,7 +14299,7 @@
         <v>144</v>
       </c>
       <c r="S145" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Karoon Arti Radhasoami Tan Man Surat Lagay.mp4</v>
       </c>
       <c r="T145" t="str">
@@ -14259,11 +14307,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U145" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Karoon Arti Radhasoami Tan Man Surat Lagay.mp4' where Shabd1_ID = 1557</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1560</v>
       </c>
@@ -14310,7 +14358,7 @@
         <v>145</v>
       </c>
       <c r="S146" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>Video/Poetry/Karoon Bandagi Radhasoami Aage.mp4</v>
       </c>
       <c r="T146" t="str">
@@ -14318,11 +14366,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U146" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Karoon Bandagi Radhasoami Aage.mp4' where Shabd1_ID = 1560</v>
       </c>
     </row>
-    <row r="147" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <v>1562</v>
       </c>
@@ -14372,8 +14420,15 @@
         <f>IF(COUNTIF(R2:R295, C147), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="148" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U147" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="V147" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U147,".mp4' where Shabd1_ID = ",A147)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Premin Door Desh Se Aaee.mp4' where Shabd1_ID = 1562</v>
+      </c>
+    </row>
+    <row r="148" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1563</v>
       </c>
@@ -14420,19 +14475,18 @@
         <v>147</v>
       </c>
       <c r="S148" t="str">
-        <f t="shared" ref="S148:S162" si="28">_xlfn.CONCAT("Video/Poetry/",R148,".mp4")</f>
+        <f t="shared" ref="S148:S162" si="26">_xlfn.CONCAT("Video/Poetry/",R148,".mp4")</f>
         <v>Video/Poetry/Karoon Binti Radhasoami Aage.mp4</v>
       </c>
       <c r="T148" t="str">
         <f>IF(COUNTIF(R2:R295, C148), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>To be linked in DB</v>
       </c>
-      <c r="U148" t="str">
-        <f t="shared" ref="U148:U162" si="29">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S148,"' where Shabd1_ID = ",A148)</f>
-        <v>update Shabd_Table set videoLink = 'Video/Poetry/Karoon Binti Radhasoami Aage.mp4' where Shabd1_ID = 1563</v>
-      </c>
-    </row>
-    <row r="149" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U148" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="149" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>1565</v>
       </c>
@@ -14479,7 +14533,7 @@
         <v>148</v>
       </c>
       <c r="S149" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Karoon Binti Radhasoami Aaj.mp4</v>
       </c>
       <c r="T149" t="str">
@@ -14487,11 +14541,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U149" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="U148:U162" si="27">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S149,"' where Shabd1_ID = ",A149)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Karoon Binti Radhasoami Aaj.mp4' where Shabd1_ID = 1565</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1572</v>
       </c>
@@ -14538,7 +14592,7 @@
         <v>149</v>
       </c>
       <c r="S150" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Kas Preetam Se Jay Miloon Main.mp4</v>
       </c>
       <c r="T150" t="str">
@@ -14546,11 +14600,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U150" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kas Preetam Se Jay Miloon Main.mp4' where Shabd1_ID = 1572</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1577</v>
       </c>
@@ -14597,7 +14651,7 @@
         <v>150</v>
       </c>
       <c r="S151" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Katik Mas Panchwa Chala.mp4</v>
       </c>
       <c r="T151" t="str">
@@ -14605,11 +14659,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U151" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Katik Mas Panchwa Chala.mp4' where Shabd1_ID = 1577</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1583</v>
       </c>
@@ -14656,7 +14710,7 @@
         <v>151</v>
       </c>
       <c r="S152" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Kaun Kare Aarat Satguru Ki.mp4</v>
       </c>
       <c r="T152" t="str">
@@ -14664,11 +14718,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U152" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kaun Kare Aarat Satguru Ki.mp4' where Shabd1_ID = 1583</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1592</v>
       </c>
@@ -14715,7 +14769,7 @@
         <v>152</v>
       </c>
       <c r="S153" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Kaya Nagar Mein Dhoom Machi Hai.mp4</v>
       </c>
       <c r="T153" t="str">
@@ -14723,11 +14777,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U153" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kaya Nagar Mein Dhoom Machi Hai.mp4' where Shabd1_ID = 1592</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1649</v>
       </c>
@@ -14774,7 +14828,7 @@
         <v>153</v>
       </c>
       <c r="S154" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Khel Rahi Surat Phaag Naee.mp4</v>
       </c>
       <c r="T154" t="str">
@@ -14782,11 +14836,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U154" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Khel Rahi Surat Phaag Naee.mp4' where Shabd1_ID = 1649</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1650</v>
       </c>
@@ -14833,7 +14887,7 @@
         <v>154</v>
       </c>
       <c r="S155" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Khila Mere Ghat Mein Aaj Basant.mp4</v>
       </c>
       <c r="T155" t="str">
@@ -14841,11 +14895,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U155" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Khila Mere Ghat Mein Aaj Basant.mp4' where Shabd1_ID = 1650</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1661</v>
       </c>
@@ -14892,7 +14946,7 @@
         <v>155</v>
       </c>
       <c r="S156" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Koi Chalo Guru Sang Agam Nagar.mp4</v>
       </c>
       <c r="T156" t="str">
@@ -14900,11 +14954,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U156" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Koi Chalo Guru Sang Agam Nagar.mp4' where Shabd1_ID = 1661</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1667</v>
       </c>
@@ -14951,7 +15005,7 @@
         <v>156</v>
       </c>
       <c r="S157" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Koi Din Ka Hai Jag Mein Rahna Sakhi.mp4</v>
       </c>
       <c r="T157" t="str">
@@ -14959,11 +15013,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U157" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Koi Din Ka Hai Jag Mein Rahna Sakhi.mp4' where Shabd1_ID = 1667</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1672</v>
       </c>
@@ -15010,7 +15064,7 @@
         <v>157</v>
       </c>
       <c r="S158" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Koi Gaho Guru Ki Saran Samhar.mp4</v>
       </c>
       <c r="T158" t="str">
@@ -15018,11 +15072,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Koi Gaho Guru Ki Saran Samhar.mp4' where Shabd1_ID = 1672</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1674</v>
       </c>
@@ -15069,7 +15123,7 @@
         <v>158</v>
       </c>
       <c r="S159" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Koi Karo Guru Ka Satsang Aaj.mp4</v>
       </c>
       <c r="T159" t="str">
@@ -15077,11 +15131,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U159" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Koi Karo Guru Ka Satsang Aaj.mp4' where Shabd1_ID = 1674</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1676</v>
       </c>
@@ -15128,7 +15182,7 @@
         <v>159</v>
       </c>
       <c r="S160" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Koi Milo Purush Se Chal Satpur.mp4</v>
       </c>
       <c r="T160" t="str">
@@ -15136,11 +15190,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U160" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Koi Milo Purush Se Chal Satpur.mp4' where Shabd1_ID = 1676</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1677</v>
       </c>
@@ -15187,7 +15241,7 @@
         <v>160</v>
       </c>
       <c r="S161" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Kya Sowe Jag Mein Nind Bhari.mp4</v>
       </c>
       <c r="T161" t="str">
@@ -15195,11 +15249,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U161" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kya Sowe Jag Mein Nind Bhari.mp4' where Shabd1_ID = 1677</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1679</v>
       </c>
@@ -15246,7 +15300,7 @@
         <v>161</v>
       </c>
       <c r="S162" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>Video/Poetry/Kyon Ghabrao Pran Piyari.mp4</v>
       </c>
       <c r="T162" t="str">
@@ -15254,11 +15308,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U162" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Kyon Ghabrao Pran Piyari.mp4' where Shabd1_ID = 1679</v>
       </c>
     </row>
-    <row r="163" spans="1:21" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:22" s="9" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <v>1680</v>
       </c>
@@ -15308,8 +15362,15 @@
         <f>IF(COUNTIF(R2:R295, C163), "To be linked in DB", "Not uploaded/created yet")</f>
         <v>Not uploaded/created yet</v>
       </c>
-    </row>
-    <row r="164" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U163" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="V163" s="9" t="str">
+        <f>_xlfn.CONCAT("update Shabd_Table set videoLink = 'Video/Poetry/",U163,".mp4' where Shabd1_ID = ",A163)</f>
+        <v>update Shabd_Table set videoLink = 'Video/Poetry/Sawan Mas Suhagin Aaee.mp4' where Shabd1_ID = 1680</v>
+      </c>
+    </row>
+    <row r="164" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1681</v>
       </c>
@@ -15356,7 +15417,7 @@
         <v>163</v>
       </c>
       <c r="S164" t="str">
-        <f t="shared" ref="S164:S169" si="30">_xlfn.CONCAT("Video/Poetry/",R164,".mp4")</f>
+        <f t="shared" ref="S164:S169" si="28">_xlfn.CONCAT("Video/Poetry/",R164,".mp4")</f>
         <v>Video/Poetry/Lagao Meri Naiya Satguru Par.mp4</v>
       </c>
       <c r="T164" t="str">
@@ -15364,11 +15425,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U164" t="str">
-        <f t="shared" ref="U164:U169" si="31">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S164,"' where Shabd1_ID = ",A164)</f>
+        <f t="shared" ref="U164:U169" si="29">_xlfn.CONCAT("update Shabd_Table set videoLink = '",S164,"' where Shabd1_ID = ",A164)</f>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Lagao Meri Naiya Satguru Par.mp4' where Shabd1_ID = 1681</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1682</v>
       </c>
@@ -15415,7 +15476,7 @@
         <v>164</v>
       </c>
       <c r="S165" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>Video/Poetry/Laj Meri Rakho Guru Maharaj.mp4</v>
       </c>
       <c r="T165" t="str">
@@ -15423,11 +15484,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U165" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Laj Meri Rakho Guru Maharaj.mp4' where Shabd1_ID = 1682</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1685</v>
       </c>
@@ -15474,7 +15535,7 @@
         <v>165</v>
       </c>
       <c r="S166" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>Video/Poetry/Main Guru Pyare Ke Charnon Ki Dasi.mp4</v>
       </c>
       <c r="T166" t="str">
@@ -15482,11 +15543,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U166" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Main Guru Pyare Ke Charnon Ki Dasi.mp4' where Shabd1_ID = 1685</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1702</v>
       </c>
@@ -15530,7 +15591,7 @@
         <v>166</v>
       </c>
       <c r="S167" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>Video/Poetry/Main Hui Sakhi Apne Pyare Ki Pyari.mp4</v>
       </c>
       <c r="T167" t="str">
@@ -15538,11 +15599,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U167" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Main Hui Sakhi Apne Pyare Ki Pyari.mp4' where Shabd1_ID = 1702</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1711</v>
       </c>
@@ -15589,7 +15650,7 @@
         <v>167</v>
       </c>
       <c r="S168" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>Video/Poetry/Main Satguru Sang Karoongi Arti.mp4</v>
       </c>
       <c r="T168" t="str">
@@ -15597,11 +15658,11 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U168" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Main Satguru Sang Karoongi Arti.mp4' where Shabd1_ID = 1711</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1713</v>
       </c>
@@ -15648,7 +15709,7 @@
         <v>168</v>
       </c>
       <c r="S169" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>Video/Poetry/Main To Holi Khelan Ko Thadhi.mp4</v>
       </c>
       <c r="T169" t="str">
@@ -15656,41 +15717,41 @@
         <v>To be linked in DB</v>
       </c>
       <c r="U169" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>update Shabd_Table set videoLink = 'Video/Poetry/Main To Holi Khelan Ko Thadhi.mp4' where Shabd1_ID = 1713</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R170" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R171" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R172" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R173" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R174" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R175" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:22" ht="19" hidden="1" x14ac:dyDescent="0.25">
       <c r="R176" s="7" t="s">
         <v>175</v>
       </c>
@@ -16306,7 +16367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39EDF73-6DE1-044A-B677-513F685FEE78}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>

</xml_diff>